<commit_message>
Now I need to comment the hell out of this, and clean some of these hack-assed scripts I used to generate data
</commit_message>
<xml_diff>
--- a/processedFiles/dataTotalsModel1.xlsx
+++ b/processedFiles/dataTotalsModel1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
   <si>
     <t>File</t>
   </si>
@@ -262,13 +262,37 @@
   </si>
   <si>
     <t>MIN</t>
+  </si>
+  <si>
+    <t>Ereg</t>
+  </si>
+  <si>
+    <t>Ep1</t>
+  </si>
+  <si>
+    <t>Ep2</t>
+  </si>
+  <si>
+    <t>Enp</t>
+  </si>
+  <si>
+    <t>Epsi</t>
+  </si>
+  <si>
+    <t>Ephi</t>
+  </si>
+  <si>
+    <t>Esa</t>
+  </si>
+  <si>
+    <t>Best Z Score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -298,13 +322,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -316,7 +360,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -326,22 +370,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -349,86 +412,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -479,26 +462,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -829,20 +792,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="84.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="5" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -894,8 +855,29 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" t="s">
+        <v>82</v>
+      </c>
+      <c r="T1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -947,8 +929,29 @@
       <c r="Q2">
         <v>0.62665636363599997</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2">
+        <v>3.97265625</v>
+      </c>
+      <c r="S2">
+        <v>0.31738281000000002</v>
+      </c>
+      <c r="T2">
+        <v>3.7421875</v>
+      </c>
+      <c r="U2">
+        <v>0.16113280999999999</v>
+      </c>
+      <c r="V2">
+        <v>7.421875E-2</v>
+      </c>
+      <c r="W2">
+        <v>1.02636719</v>
+      </c>
+      <c r="X2">
+        <v>0.45605468999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1000,8 +1003,29 @@
       <c r="Q3">
         <v>0.63351363636400004</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3">
+        <v>2.7529296900000002</v>
+      </c>
+      <c r="S3">
+        <v>0.57910156000000002</v>
+      </c>
+      <c r="T3">
+        <v>1.72558594</v>
+      </c>
+      <c r="U3">
+        <v>0.6328125</v>
+      </c>
+      <c r="V3">
+        <v>0.13867188</v>
+      </c>
+      <c r="W3">
+        <v>0.68847656000000002</v>
+      </c>
+      <c r="X3">
+        <v>0.37402343999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -1053,8 +1077,29 @@
       <c r="Q4">
         <v>0.62666999999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4">
+        <v>3.87890625</v>
+      </c>
+      <c r="S4">
+        <v>0.17382812</v>
+      </c>
+      <c r="T4">
+        <v>3.12304688</v>
+      </c>
+      <c r="U4">
+        <v>2.328125</v>
+      </c>
+      <c r="V4">
+        <v>0.24609375</v>
+      </c>
+      <c r="W4">
+        <v>0.99804687999999997</v>
+      </c>
+      <c r="X4">
+        <v>0.39453125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1106,8 +1151,29 @@
       <c r="Q5">
         <v>0.62510454545500005</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5">
+        <v>3.71679688</v>
+      </c>
+      <c r="S5">
+        <v>0.44824218999999998</v>
+      </c>
+      <c r="T5">
+        <v>3.5107421900000002</v>
+      </c>
+      <c r="U5">
+        <v>0.73144531000000002</v>
+      </c>
+      <c r="V5">
+        <v>1.7578119999999999E-2</v>
+      </c>
+      <c r="W5">
+        <v>0.84082031000000002</v>
+      </c>
+      <c r="X5">
+        <v>0.37304688000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1159,8 +1225,29 @@
       <c r="Q6">
         <v>0.62867272727300005</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6" s="1">
+        <v>3.14648438</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0.91308593800000004</v>
+      </c>
+      <c r="T6" s="1">
+        <v>1.18066406</v>
+      </c>
+      <c r="U6" s="1">
+        <v>2.11132812</v>
+      </c>
+      <c r="V6" s="1">
+        <v>2.9296875E-3</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0.775390625</v>
+      </c>
+      <c r="X6" s="1">
+        <v>0.40917968799999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1212,8 +1299,29 @@
       <c r="Q7">
         <v>0.61971545454499999</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7">
+        <v>3.21289062</v>
+      </c>
+      <c r="S7">
+        <v>7.03125E-2</v>
+      </c>
+      <c r="T7">
+        <v>3.94335938</v>
+      </c>
+      <c r="U7">
+        <v>0.68847656000000002</v>
+      </c>
+      <c r="V7">
+        <v>8.6914060000000001E-2</v>
+      </c>
+      <c r="W7">
+        <v>0.55859375</v>
+      </c>
+      <c r="X7">
+        <v>0.24316405999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1265,8 +1373,29 @@
       <c r="Q8">
         <v>0.61949181818200005</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8">
+        <v>3.65625</v>
+      </c>
+      <c r="S8">
+        <v>0.48144531000000002</v>
+      </c>
+      <c r="T8">
+        <v>2.75976562</v>
+      </c>
+      <c r="U8">
+        <v>1.796875</v>
+      </c>
+      <c r="V8">
+        <v>0.15917969000000001</v>
+      </c>
+      <c r="W8">
+        <v>0.64453125</v>
+      </c>
+      <c r="X8">
+        <v>0.28710938000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1318,8 +1447,29 @@
       <c r="Q9">
         <v>0.62062454545500001</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9">
+        <v>3.76367188</v>
+      </c>
+      <c r="S9">
+        <v>0.54492187999999997</v>
+      </c>
+      <c r="T9">
+        <v>2.99609375</v>
+      </c>
+      <c r="U9">
+        <v>1.4765625</v>
+      </c>
+      <c r="V9">
+        <v>0.14355469000000001</v>
+      </c>
+      <c r="W9">
+        <v>0.64550781000000002</v>
+      </c>
+      <c r="X9">
+        <v>0.24316405999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -1371,8 +1521,29 @@
       <c r="Q10">
         <v>0.62640818181799995</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10">
+        <v>3.21484375</v>
+      </c>
+      <c r="S10">
+        <v>1.34863281</v>
+      </c>
+      <c r="T10">
+        <v>1.70507812</v>
+      </c>
+      <c r="U10">
+        <v>0.66210937999999997</v>
+      </c>
+      <c r="V10">
+        <v>2.1484380000000001E-2</v>
+      </c>
+      <c r="W10">
+        <v>0.98730468999999998</v>
+      </c>
+      <c r="X10">
+        <v>0.30761718999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1424,8 +1595,29 @@
       <c r="Q11">
         <v>0.62678727272699997</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11">
+        <v>3.9873046900000002</v>
+      </c>
+      <c r="S11">
+        <v>1.33398438</v>
+      </c>
+      <c r="T11">
+        <v>3.71484375</v>
+      </c>
+      <c r="U11">
+        <v>1.0546875</v>
+      </c>
+      <c r="V11">
+        <v>5.3710939999999999E-2</v>
+      </c>
+      <c r="W11">
+        <v>1.15136719</v>
+      </c>
+      <c r="X11">
+        <v>0.48144531000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1477,8 +1669,29 @@
       <c r="Q12">
         <v>0.62288545454499999</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" s="1">
+        <v>3.3427734400000002</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0.451171875</v>
+      </c>
+      <c r="T12" s="1">
+        <v>3.9111328099999998</v>
+      </c>
+      <c r="U12" s="1">
+        <v>2.73046875</v>
+      </c>
+      <c r="V12" s="1">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.859375</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0.380859375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1530,8 +1743,29 @@
       <c r="Q13">
         <v>0.62902727272699999</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13">
+        <v>3.6357421900000002</v>
+      </c>
+      <c r="S13">
+        <v>1.25292969</v>
+      </c>
+      <c r="T13">
+        <v>3.8759765599999998</v>
+      </c>
+      <c r="U13">
+        <v>1.73046875</v>
+      </c>
+      <c r="V13">
+        <v>5.85938E-3</v>
+      </c>
+      <c r="W13">
+        <v>0.82617187999999997</v>
+      </c>
+      <c r="X13">
+        <v>0.48339843999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1583,8 +1817,29 @@
       <c r="Q14">
         <v>0.627080909091</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14">
+        <v>3.5830078099999998</v>
+      </c>
+      <c r="S14">
+        <v>1.97460938</v>
+      </c>
+      <c r="T14">
+        <v>2.703125</v>
+      </c>
+      <c r="U14">
+        <v>1.9765625</v>
+      </c>
+      <c r="V14">
+        <v>1.269531E-2</v>
+      </c>
+      <c r="W14">
+        <v>0.73730468999999998</v>
+      </c>
+      <c r="X14">
+        <v>0.44433593999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1636,8 +1891,29 @@
       <c r="Q15">
         <v>0.62794181818200001</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15">
+        <v>3.5087890599999998</v>
+      </c>
+      <c r="S15">
+        <v>1.90136719</v>
+      </c>
+      <c r="T15">
+        <v>3.5595703099999998</v>
+      </c>
+      <c r="U15">
+        <v>1.07226562</v>
+      </c>
+      <c r="V15">
+        <v>0.15722655999999999</v>
+      </c>
+      <c r="W15">
+        <v>0.82324218999999998</v>
+      </c>
+      <c r="X15">
+        <v>0.45996093999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1689,8 +1965,29 @@
       <c r="Q16">
         <v>0.63480272727300002</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16">
+        <v>3.90234375</v>
+      </c>
+      <c r="S16">
+        <v>3.0283203099999998</v>
+      </c>
+      <c r="T16">
+        <v>3.03320312</v>
+      </c>
+      <c r="U16">
+        <v>0.47363281000000002</v>
+      </c>
+      <c r="V16">
+        <v>1.269531E-2</v>
+      </c>
+      <c r="W16">
+        <v>0.95019531000000002</v>
+      </c>
+      <c r="X16">
+        <v>0.59570312000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1742,8 +2039,29 @@
       <c r="Q17">
         <v>0.62843090909099997</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="R17">
+        <v>3.5869140599999998</v>
+      </c>
+      <c r="S17">
+        <v>2.7958984400000002</v>
+      </c>
+      <c r="T17">
+        <v>2.3251953099999998</v>
+      </c>
+      <c r="U17">
+        <v>0.421875</v>
+      </c>
+      <c r="V17">
+        <v>1.8554689999999999E-2</v>
+      </c>
+      <c r="W17">
+        <v>0.95898437999999997</v>
+      </c>
+      <c r="X17">
+        <v>0.46484375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1795,8 +2113,29 @@
       <c r="Q18">
         <v>0.62523909090899998</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="R18">
+        <v>3.7705078099999998</v>
+      </c>
+      <c r="S18">
+        <v>2.1015625</v>
+      </c>
+      <c r="T18">
+        <v>1.79003906</v>
+      </c>
+      <c r="U18">
+        <v>3.5712890599999998</v>
+      </c>
+      <c r="V18">
+        <v>2.5390619999999999E-2</v>
+      </c>
+      <c r="W18">
+        <v>0.96289062000000003</v>
+      </c>
+      <c r="X18">
+        <v>0.37988281000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1848,8 +2187,29 @@
       <c r="Q19">
         <v>0.61702363636400004</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="R19">
+        <v>2.7705078099999998</v>
+      </c>
+      <c r="S19">
+        <v>1.53320312</v>
+      </c>
+      <c r="T19">
+        <v>1.40332031</v>
+      </c>
+      <c r="U19">
+        <v>1.99609375</v>
+      </c>
+      <c r="V19">
+        <v>9.8632810000000001E-2</v>
+      </c>
+      <c r="W19">
+        <v>0.50878906000000002</v>
+      </c>
+      <c r="X19">
+        <v>0.20117188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1901,8 +2261,29 @@
       <c r="Q20">
         <v>0.61716636363599997</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="R20">
+        <v>2.375</v>
+      </c>
+      <c r="S20">
+        <v>1.09179688</v>
+      </c>
+      <c r="T20">
+        <v>3.66796875</v>
+      </c>
+      <c r="U20">
+        <v>0.4453125</v>
+      </c>
+      <c r="V20">
+        <v>8.7890599999999996E-3</v>
+      </c>
+      <c r="W20">
+        <v>0.51171875</v>
+      </c>
+      <c r="X20">
+        <v>0.24414062</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1954,8 +2335,29 @@
       <c r="Q21">
         <v>0.62057636363599999</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" s="1">
+        <v>3.7705078099999998</v>
+      </c>
+      <c r="S21" s="1">
+        <v>2.79882812</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0.984375</v>
+      </c>
+      <c r="U21" s="1">
+        <v>3.19335938</v>
+      </c>
+      <c r="V21" s="1">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="W21" s="1">
+        <v>1.03710938</v>
+      </c>
+      <c r="X21" s="1">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2007,8 +2409,29 @@
       <c r="Q22">
         <v>0.62632454545500005</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="R22">
+        <v>2.82226562</v>
+      </c>
+      <c r="S22">
+        <v>1.40527344</v>
+      </c>
+      <c r="T22">
+        <v>3.36523438</v>
+      </c>
+      <c r="U22">
+        <v>2.14648438</v>
+      </c>
+      <c r="V22">
+        <v>0.13867188</v>
+      </c>
+      <c r="W22">
+        <v>0.56542968999999998</v>
+      </c>
+      <c r="X22">
+        <v>0.27636718999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -2060,8 +2483,29 @@
       <c r="Q23">
         <v>0.62142636363600001</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="R23">
+        <v>3.08984375</v>
+      </c>
+      <c r="S23">
+        <v>2.4775390599999998</v>
+      </c>
+      <c r="T23">
+        <v>0.96777343999999998</v>
+      </c>
+      <c r="U23">
+        <v>1.62402344</v>
+      </c>
+      <c r="V23">
+        <v>3.90625E-2</v>
+      </c>
+      <c r="W23">
+        <v>0.74414062000000003</v>
+      </c>
+      <c r="X23">
+        <v>0.23925780999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2113,8 +2557,29 @@
       <c r="Q24">
         <v>0.63273999999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="R24">
+        <v>3.16210938</v>
+      </c>
+      <c r="S24">
+        <v>3.46875</v>
+      </c>
+      <c r="T24">
+        <v>0.90820312000000003</v>
+      </c>
+      <c r="U24">
+        <v>0.56738281000000002</v>
+      </c>
+      <c r="V24">
+        <v>4.3945310000000001E-2</v>
+      </c>
+      <c r="W24">
+        <v>0.55371093999999998</v>
+      </c>
+      <c r="X24">
+        <v>0.38769531000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2166,8 +2631,29 @@
       <c r="Q25">
         <v>0.62760727272700001</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="R25">
+        <v>3.5869140599999998</v>
+      </c>
+      <c r="S25">
+        <v>3.66210938</v>
+      </c>
+      <c r="T25">
+        <v>3.64257812</v>
+      </c>
+      <c r="U25">
+        <v>0.34667968999999998</v>
+      </c>
+      <c r="V25">
+        <v>3.515625E-2</v>
+      </c>
+      <c r="W25">
+        <v>0.81640625</v>
+      </c>
+      <c r="X25">
+        <v>0.47167968999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2219,8 +2705,29 @@
       <c r="Q26">
         <v>0.625821818182</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="R26">
+        <v>3.71679688</v>
+      </c>
+      <c r="S26">
+        <v>3.9375</v>
+      </c>
+      <c r="T26">
+        <v>2.3798828099999998</v>
+      </c>
+      <c r="U26">
+        <v>0.28027343999999998</v>
+      </c>
+      <c r="V26">
+        <v>6.25E-2</v>
+      </c>
+      <c r="W26">
+        <v>0.94042968999999998</v>
+      </c>
+      <c r="X26">
+        <v>0.39648438000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -2272,8 +2779,29 @@
       <c r="Q27">
         <v>0.62970454545499999</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="R27">
+        <v>3.12695312</v>
+      </c>
+      <c r="S27">
+        <v>2.7353515599999998</v>
+      </c>
+      <c r="T27">
+        <v>3.33398438</v>
+      </c>
+      <c r="U27">
+        <v>1.75</v>
+      </c>
+      <c r="V27">
+        <v>6.0546879999999997E-2</v>
+      </c>
+      <c r="W27">
+        <v>0.83007812000000003</v>
+      </c>
+      <c r="X27">
+        <v>0.35644531000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2325,8 +2853,29 @@
       <c r="Q28">
         <v>0.62285636363600005</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="R28">
+        <v>3.7412109400000002</v>
+      </c>
+      <c r="S28">
+        <v>3.40234375</v>
+      </c>
+      <c r="T28">
+        <v>3.2197265599999998</v>
+      </c>
+      <c r="U28">
+        <v>3.00976562</v>
+      </c>
+      <c r="V28">
+        <v>4.296875E-2</v>
+      </c>
+      <c r="W28">
+        <v>0.85253906000000002</v>
+      </c>
+      <c r="X28">
+        <v>0.40332031000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -2378,8 +2927,29 @@
       <c r="Q29">
         <v>0.62189727272700002</v>
       </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29">
+        <v>3.37109375</v>
+      </c>
+      <c r="S29">
+        <v>3.42773438</v>
+      </c>
+      <c r="T29">
+        <v>2.9716796900000002</v>
+      </c>
+      <c r="U29">
+        <v>0.171875</v>
+      </c>
+      <c r="V29">
+        <v>4.0039060000000001E-2</v>
+      </c>
+      <c r="W29">
+        <v>0.875</v>
+      </c>
+      <c r="X29">
+        <v>0.30566406000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -2431,8 +3001,29 @@
       <c r="Q30">
         <v>0.62031727272699999</v>
       </c>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="R30">
+        <v>3.11523438</v>
+      </c>
+      <c r="S30">
+        <v>3.58007812</v>
+      </c>
+      <c r="T30">
+        <v>3.4482421900000002</v>
+      </c>
+      <c r="U30">
+        <v>0.52246093999999998</v>
+      </c>
+      <c r="V30">
+        <v>7.5195310000000001E-2</v>
+      </c>
+      <c r="W30">
+        <v>0.26660156000000002</v>
+      </c>
+      <c r="X30">
+        <v>0.28222656000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -2484,8 +3075,29 @@
       <c r="Q31">
         <v>0.62293363636400001</v>
       </c>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="R31">
+        <v>1.8671875</v>
+      </c>
+      <c r="S31">
+        <v>2.7021484400000002</v>
+      </c>
+      <c r="T31">
+        <v>2.97070312</v>
+      </c>
+      <c r="U31">
+        <v>9.6679689999999999E-2</v>
+      </c>
+      <c r="V31">
+        <v>8.3984379999999997E-2</v>
+      </c>
+      <c r="W31">
+        <v>0.46386718999999998</v>
+      </c>
+      <c r="X31">
+        <v>0.22363280999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2549,8 +3161,36 @@
         <f t="shared" si="0"/>
         <v>0.62518160606060003</v>
       </c>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="R33">
+        <f t="shared" ref="R33:X33" si="1">AVERAGE(R2:R31)</f>
+        <v>3.3716145836666667</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>1.8646484377666666</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="1"/>
+        <v>2.7621093743333334</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="1"/>
+        <v>1.3256835936666671</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="1"/>
+        <v>6.3606771083333319E-2</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="1"/>
+        <v>0.7800130211666666</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="1"/>
+        <v>0.36263020843333327</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -2559,63 +3199,91 @@
         <v>0.50126426456483686</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:Q34" si="1">STDEV(D2:D31)</f>
+        <f t="shared" ref="D34:Q34" si="2">STDEV(D2:D31)</f>
         <v>8.2963404559285268E-3</v>
       </c>
       <c r="E34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0632154973493511E-3</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.23789382453484637</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.186578947174131E-3</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7640748696548274E-3</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7770382224360953E-2</v>
       </c>
       <c r="J34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0872808022616737E-3</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4394491711838607E-3</v>
       </c>
       <c r="L34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0323859389758689</v>
       </c>
       <c r="M34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.6038501632254632E-3</v>
       </c>
       <c r="N34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4963797026125493E-3</v>
       </c>
       <c r="O34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.74665594415695247</v>
       </c>
       <c r="P34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4676293612784533E-3</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5626872690732127E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="R34">
+        <f t="shared" ref="R34:X34" si="3">STDEV(R2:R31)</f>
+        <v>0.49430442791607515</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="3"/>
+        <v>1.2230530614987922</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="3"/>
+        <v>0.98216900276100283</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="3"/>
+        <v>0.99640178320389539</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="3"/>
+        <v>6.0061938960045129E-2</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="3"/>
+        <v>0.20433303468540315</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="3"/>
+        <v>9.637403583551768E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -2624,63 +3292,91 @@
         <v>-3.3340074500000001</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:Q35" si="2">MAX(D2:D31)</f>
+        <f t="shared" ref="D35:Q35" si="4">MAX(D2:D31)</f>
         <v>-0.64881883673200003</v>
       </c>
       <c r="E35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.68342499999999995</v>
       </c>
       <c r="F35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.3171849899999999</v>
       </c>
       <c r="G35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.90926767685700005</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.77912999999999999</v>
       </c>
       <c r="I35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.58689765</v>
       </c>
       <c r="J35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.46803021554399998</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.54593275862099999</v>
       </c>
       <c r="L35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3.33203753</v>
       </c>
       <c r="M35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.50345626459299997</v>
       </c>
       <c r="N35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.585319642857</v>
       </c>
       <c r="O35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-6.0142389500000002</v>
       </c>
       <c r="P35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.62340734065100001</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.63480272727300002</v>
       </c>
-    </row>
-    <row r="36" spans="1:17">
+      <c r="R35">
+        <f t="shared" ref="R35:X35" si="5">MAX(R2:R31)</f>
+        <v>3.9873046900000002</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="5"/>
+        <v>3.9375</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="5"/>
+        <v>3.94335938</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="5"/>
+        <v>3.5712890599999998</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="5"/>
+        <v>0.24609375</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="5"/>
+        <v>1.15136719</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="5"/>
+        <v>0.59570312000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -2689,89 +3385,196 @@
         <v>-5.2326664999999997</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:Q36" si="3">MIN(D2:D31)</f>
+        <f t="shared" ref="D36:Q36" si="6">MIN(D2:D31)</f>
         <v>-0.68088681563300002</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.67475564516099995</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.2838755399999999</v>
       </c>
       <c r="G36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.91772524156500002</v>
       </c>
       <c r="H36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.76847500000000002</v>
       </c>
       <c r="I36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.7162569200000002</v>
       </c>
       <c r="J36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.48046895267500001</v>
       </c>
       <c r="K36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.53443793103399995</v>
       </c>
       <c r="L36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-7.09643815</v>
       </c>
       <c r="M36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.53890967628099995</v>
       </c>
       <c r="N36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.57015357142900003</v>
       </c>
       <c r="O36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-8.8992153900000002</v>
       </c>
       <c r="P36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.58528258881100004</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.61702363636400004</v>
+      </c>
+      <c r="R36">
+        <f t="shared" ref="R36:X36" si="7">MIN(R2:R31)</f>
+        <v>1.8671875</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="7"/>
+        <v>7.03125E-2</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="7"/>
+        <v>0.90820312000000003</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="7"/>
+        <v>9.6679689999999999E-2</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="7"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="7"/>
+        <v>0.26660156000000002</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="7"/>
+        <v>0.20117188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24">
+      <c r="A39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="3">
+        <v>-3.3340074500000001</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="2">
+        <v>-0.67286175500000001</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.67818064499999997</v>
+      </c>
+      <c r="F39" s="2">
+        <v>-1.3603195699999999</v>
+      </c>
+      <c r="G39" s="2">
+        <v>-0.91460094999999997</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.773505</v>
+      </c>
+      <c r="I39" s="2">
+        <v>-2.6294337400000001</v>
+      </c>
+      <c r="J39" s="2">
+        <v>-0.479670294</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0.54121724100000002</v>
+      </c>
+      <c r="L39" s="2">
+        <v>-3.33203753</v>
+      </c>
+      <c r="M39" s="2">
+        <v>-0.51226121000000002</v>
+      </c>
+      <c r="N39" s="2">
+        <v>0.58121428600000002</v>
+      </c>
+      <c r="O39" s="2">
+        <v>-6.0142389500000002</v>
+      </c>
+      <c r="P39" s="2">
+        <v>0.61186147599999996</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>0.62665636400000002</v>
+      </c>
+      <c r="R39" s="2">
+        <v>3.97265625</v>
+      </c>
+      <c r="S39" s="2">
+        <v>0.31738281000000002</v>
+      </c>
+      <c r="T39" s="2">
+        <v>3.7421875</v>
+      </c>
+      <c r="U39" s="2">
+        <v>0.16113280999999999</v>
+      </c>
+      <c r="V39" s="2">
+        <v>7.421875E-2</v>
+      </c>
+      <c r="W39" s="2">
+        <v>1.02636719</v>
+      </c>
+      <c r="X39" s="2">
+        <v>0.45605468999999998</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:Q31">
-    <sortCondition descending="1" ref="B2:B31"/>
+    <sortCondition descending="1" ref="A2:A31"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:B31">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>$B$36</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>$B$35</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D31">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$D$36</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>$D$35</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E31">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>$E$36</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$E$35</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>$E$36</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>